<commit_message>
total count job valid history
</commit_message>
<xml_diff>
--- a/3_extract/count_history_index.xlsx
+++ b/3_extract/count_history_index.xlsx
@@ -442,7 +442,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -487,7 +487,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -517,7 +517,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -547,7 +547,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -557,7 +557,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
@@ -577,7 +577,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -622,7 +622,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -637,7 +637,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>20</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42">
@@ -652,7 +652,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -667,12 +667,12 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49">
@@ -697,7 +697,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -707,12 +707,12 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -732,7 +732,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61">
@@ -747,7 +747,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -762,7 +762,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -777,7 +777,7 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -787,7 +787,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72">
@@ -817,7 +817,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78">
@@ -832,7 +832,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81">
@@ -852,12 +852,12 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -867,7 +867,7 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88">
@@ -882,7 +882,7 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
@@ -942,12 +942,12 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -957,7 +957,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106">
@@ -987,7 +987,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112">
@@ -1017,7 +1017,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118">
@@ -1037,7 +1037,7 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -1047,7 +1047,7 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -1057,7 +1057,7 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126">
@@ -1087,7 +1087,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132">
@@ -1097,12 +1097,12 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135">
@@ -1122,7 +1122,7 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139">
@@ -1157,7 +1157,7 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146">
@@ -1197,7 +1197,7 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154">
@@ -1232,7 +1232,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -1252,12 +1252,12 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="166">
@@ -1292,17 +1292,17 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175">
@@ -1327,7 +1327,7 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180">
@@ -1352,7 +1352,7 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="185">
@@ -1367,7 +1367,7 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -1377,7 +1377,7 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190">
@@ -1392,7 +1392,7 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193">
@@ -1432,12 +1432,12 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="202">
@@ -1447,7 +1447,7 @@
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204">
@@ -1457,7 +1457,7 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="206">
@@ -1477,7 +1477,7 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="210">
@@ -1487,7 +1487,7 @@
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="212">
@@ -1497,17 +1497,17 @@
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216">
@@ -1517,17 +1517,17 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="220">
@@ -1537,7 +1537,7 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222">
@@ -1547,7 +1547,7 @@
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -1557,12 +1557,12 @@
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227">
@@ -1587,22 +1587,22 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235">
@@ -1612,12 +1612,12 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="238">
@@ -1652,7 +1652,7 @@
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="245">
@@ -1667,7 +1667,7 @@
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="248">
@@ -1682,12 +1682,12 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="252">
@@ -1712,7 +1712,7 @@
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="257">
@@ -1742,7 +1742,7 @@
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -1752,7 +1752,7 @@
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
@@ -1807,22 +1807,22 @@
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="279">
@@ -1832,7 +1832,7 @@
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="281">
@@ -1847,7 +1847,7 @@
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="284">
@@ -1862,17 +1862,17 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="289">
@@ -1907,7 +1907,7 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="296">
@@ -1942,12 +1942,12 @@
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="304">
@@ -1962,22 +1962,22 @@
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="310">
@@ -1992,17 +1992,17 @@
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="315">
@@ -2012,12 +2012,12 @@
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="318">
@@ -2027,7 +2027,7 @@
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="320">
@@ -2037,7 +2037,7 @@
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322">
@@ -2052,12 +2052,12 @@
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -2067,7 +2067,7 @@
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="328">
@@ -2082,12 +2082,12 @@
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332">
@@ -2102,7 +2102,7 @@
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="335">
@@ -2117,7 +2117,7 @@
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="338">
@@ -2127,12 +2127,12 @@
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="341">
@@ -2182,7 +2182,7 @@
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351">

</xml_diff>